<commit_message>
files organization, passport dependencies added react app initialized
</commit_message>
<xml_diff>
--- a/CronogramaProjetoFinal.xlsx
+++ b/CronogramaProjetoFinal.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22704"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EEB45DA-AFDE-4674-995E-7AA66C579EB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49C3EE9-4694-194F-8AA4-E64D64D964F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28710" windowHeight="14415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="28720" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Linha Cronológica do Projeto" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Linha Cronológica do Projeto'!$5:$6</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -165,9 +165,6 @@
     <t>Realização do módulo de autenticação e autorização (user login and register) utilizando passport e permitindo compatibilidade com os protocolos (Kerberos, openId, SAML)</t>
   </si>
   <si>
-    <t>Estudo de framework para web app (Angular)</t>
-  </si>
-  <si>
     <t>Implementação de web app para teste do módulo</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>Lançar aplicação</t>
+  </si>
+  <si>
+    <t>Estudo de framework para web app (React js)</t>
   </si>
 </sst>
 </file>
@@ -230,13 +230,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="d"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="d"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -852,7 +852,7 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" applyFill="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyBorder="0">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" applyBorder="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
@@ -861,10 +861,10 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -964,13 +964,13 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="3" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="168" fontId="22" fillId="3" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="4" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="168" fontId="22" fillId="4" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="3" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="22" fillId="3" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -994,6 +994,24 @@
     <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="9" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="6" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="44" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1008,24 +1026,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="45" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="6" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -1077,7 +1077,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Note" xfId="24" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="19" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="14" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Per cent" xfId="14" builtinId="5" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="26" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="23" builtinId="11" customBuiltin="1"/>
@@ -1557,1093 +1557,1093 @@
   </sheetPr>
   <dimension ref="B1:EN29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="EM29" sqref="EM7:EM29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="85.875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="85.83203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="2.5" style="1" customWidth="1"/>
-    <col min="4" max="17" width="2.125" style="1" customWidth="1"/>
-    <col min="18" max="142" width="2.125" customWidth="1"/>
-    <col min="143" max="143" width="17.375" style="2" customWidth="1"/>
-    <col min="144" max="144" width="2.625" customWidth="1"/>
+    <col min="4" max="17" width="2.1640625" style="1" customWidth="1"/>
+    <col min="18" max="142" width="2.1640625" customWidth="1"/>
+    <col min="143" max="143" width="17.33203125" style="2" customWidth="1"/>
+    <col min="144" max="144" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:144" ht="48.75" customHeight="1">
-      <c r="B1" s="38" t="s">
+    <row r="1" spans="2:144" ht="48.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="38"/>
-      <c r="AB1" s="38"/>
-      <c r="AC1" s="38"/>
-      <c r="AD1" s="38"/>
-      <c r="AE1" s="38"/>
-      <c r="AF1" s="38"/>
-      <c r="AG1" s="38"/>
-      <c r="AH1" s="38"/>
-      <c r="AI1" s="38"/>
-      <c r="AJ1" s="38"/>
-      <c r="AK1" s="38"/>
-      <c r="AL1" s="38"/>
-      <c r="AM1" s="38"/>
-      <c r="AN1" s="38"/>
-      <c r="AO1" s="38"/>
-      <c r="AP1" s="38"/>
-      <c r="AQ1" s="38"/>
-      <c r="AR1" s="38"/>
-      <c r="AS1" s="38"/>
-      <c r="AT1" s="38"/>
-      <c r="AU1" s="38"/>
-      <c r="AV1" s="38"/>
-      <c r="AW1" s="38"/>
-      <c r="AX1" s="38"/>
-      <c r="AY1" s="38"/>
-      <c r="AZ1" s="38"/>
-      <c r="BA1" s="38"/>
-      <c r="BB1" s="38"/>
-      <c r="BC1" s="38"/>
-      <c r="BD1" s="38"/>
-      <c r="BE1" s="38"/>
-      <c r="BF1" s="38"/>
-      <c r="BG1" s="38"/>
-      <c r="BH1" s="38"/>
-      <c r="BI1" s="38"/>
-      <c r="BJ1" s="38"/>
-      <c r="BK1" s="38"/>
-      <c r="BL1" s="38"/>
-      <c r="BM1" s="38"/>
-      <c r="BN1" s="38"/>
-      <c r="BO1" s="38"/>
-      <c r="BP1" s="38"/>
-      <c r="BQ1" s="38"/>
-      <c r="BR1" s="38"/>
-      <c r="BS1" s="38"/>
-      <c r="BT1" s="38"/>
-      <c r="BU1" s="38"/>
-      <c r="BV1" s="38"/>
-      <c r="BW1" s="38"/>
-      <c r="BX1" s="38"/>
-      <c r="BY1" s="38"/>
-      <c r="BZ1" s="38"/>
-      <c r="CA1" s="38"/>
-      <c r="CB1" s="38"/>
-      <c r="CC1" s="38"/>
-      <c r="CD1" s="38"/>
-      <c r="CE1" s="38"/>
-      <c r="CF1" s="38"/>
-      <c r="CG1" s="38"/>
-      <c r="CH1" s="38"/>
-      <c r="CI1" s="38"/>
-      <c r="CJ1" s="38"/>
-      <c r="CK1" s="38"/>
-      <c r="CL1" s="38"/>
-      <c r="CM1" s="38"/>
-      <c r="CN1" s="38"/>
-      <c r="CO1" s="38"/>
-      <c r="CP1" s="38"/>
-      <c r="CQ1" s="38"/>
-      <c r="CR1" s="38"/>
-      <c r="CS1" s="38"/>
-      <c r="CT1" s="38"/>
-      <c r="CU1" s="38"/>
-      <c r="CV1" s="38"/>
-      <c r="CW1" s="38"/>
-      <c r="CX1" s="38"/>
-      <c r="CY1" s="38"/>
-      <c r="CZ1" s="38"/>
-      <c r="DA1" s="38"/>
-      <c r="DB1" s="38"/>
-      <c r="DC1" s="38"/>
-      <c r="DD1" s="38"/>
-      <c r="DE1" s="38"/>
-      <c r="DF1" s="38"/>
-      <c r="DG1" s="38"/>
-      <c r="DH1" s="38"/>
-      <c r="DI1" s="38"/>
-      <c r="DJ1" s="38"/>
-      <c r="DK1" s="38"/>
-      <c r="DL1" s="38"/>
-      <c r="DM1" s="38"/>
-      <c r="DN1" s="38"/>
-      <c r="DO1" s="38"/>
-      <c r="DP1" s="38"/>
-      <c r="DQ1" s="38"/>
-      <c r="DR1" s="38"/>
-      <c r="DS1" s="38"/>
-      <c r="DT1" s="38"/>
-      <c r="DU1" s="38"/>
-      <c r="DV1" s="38"/>
-      <c r="DW1" s="38"/>
-      <c r="DX1" s="38"/>
-      <c r="DY1" s="38"/>
-      <c r="DZ1" s="38"/>
-      <c r="EA1" s="38"/>
-      <c r="EB1" s="38"/>
-      <c r="EC1" s="38"/>
-      <c r="ED1" s="38"/>
-      <c r="EE1" s="38"/>
-      <c r="EF1" s="38"/>
-      <c r="EG1" s="38"/>
-      <c r="EH1" s="38"/>
-      <c r="EI1" s="38"/>
-      <c r="EJ1" s="38"/>
-      <c r="EK1" s="38"/>
-      <c r="EL1" s="38"/>
-      <c r="EM1" s="38"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="31"/>
+      <c r="AQ1" s="31"/>
+      <c r="AR1" s="31"/>
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
+      <c r="AW1" s="31"/>
+      <c r="AX1" s="31"/>
+      <c r="AY1" s="31"/>
+      <c r="AZ1" s="31"/>
+      <c r="BA1" s="31"/>
+      <c r="BB1" s="31"/>
+      <c r="BC1" s="31"/>
+      <c r="BD1" s="31"/>
+      <c r="BE1" s="31"/>
+      <c r="BF1" s="31"/>
+      <c r="BG1" s="31"/>
+      <c r="BH1" s="31"/>
+      <c r="BI1" s="31"/>
+      <c r="BJ1" s="31"/>
+      <c r="BK1" s="31"/>
+      <c r="BL1" s="31"/>
+      <c r="BM1" s="31"/>
+      <c r="BN1" s="31"/>
+      <c r="BO1" s="31"/>
+      <c r="BP1" s="31"/>
+      <c r="BQ1" s="31"/>
+      <c r="BR1" s="31"/>
+      <c r="BS1" s="31"/>
+      <c r="BT1" s="31"/>
+      <c r="BU1" s="31"/>
+      <c r="BV1" s="31"/>
+      <c r="BW1" s="31"/>
+      <c r="BX1" s="31"/>
+      <c r="BY1" s="31"/>
+      <c r="BZ1" s="31"/>
+      <c r="CA1" s="31"/>
+      <c r="CB1" s="31"/>
+      <c r="CC1" s="31"/>
+      <c r="CD1" s="31"/>
+      <c r="CE1" s="31"/>
+      <c r="CF1" s="31"/>
+      <c r="CG1" s="31"/>
+      <c r="CH1" s="31"/>
+      <c r="CI1" s="31"/>
+      <c r="CJ1" s="31"/>
+      <c r="CK1" s="31"/>
+      <c r="CL1" s="31"/>
+      <c r="CM1" s="31"/>
+      <c r="CN1" s="31"/>
+      <c r="CO1" s="31"/>
+      <c r="CP1" s="31"/>
+      <c r="CQ1" s="31"/>
+      <c r="CR1" s="31"/>
+      <c r="CS1" s="31"/>
+      <c r="CT1" s="31"/>
+      <c r="CU1" s="31"/>
+      <c r="CV1" s="31"/>
+      <c r="CW1" s="31"/>
+      <c r="CX1" s="31"/>
+      <c r="CY1" s="31"/>
+      <c r="CZ1" s="31"/>
+      <c r="DA1" s="31"/>
+      <c r="DB1" s="31"/>
+      <c r="DC1" s="31"/>
+      <c r="DD1" s="31"/>
+      <c r="DE1" s="31"/>
+      <c r="DF1" s="31"/>
+      <c r="DG1" s="31"/>
+      <c r="DH1" s="31"/>
+      <c r="DI1" s="31"/>
+      <c r="DJ1" s="31"/>
+      <c r="DK1" s="31"/>
+      <c r="DL1" s="31"/>
+      <c r="DM1" s="31"/>
+      <c r="DN1" s="31"/>
+      <c r="DO1" s="31"/>
+      <c r="DP1" s="31"/>
+      <c r="DQ1" s="31"/>
+      <c r="DR1" s="31"/>
+      <c r="DS1" s="31"/>
+      <c r="DT1" s="31"/>
+      <c r="DU1" s="31"/>
+      <c r="DV1" s="31"/>
+      <c r="DW1" s="31"/>
+      <c r="DX1" s="31"/>
+      <c r="DY1" s="31"/>
+      <c r="DZ1" s="31"/>
+      <c r="EA1" s="31"/>
+      <c r="EB1" s="31"/>
+      <c r="EC1" s="31"/>
+      <c r="ED1" s="31"/>
+      <c r="EE1" s="31"/>
+      <c r="EF1" s="31"/>
+      <c r="EG1" s="31"/>
+      <c r="EH1" s="31"/>
+      <c r="EI1" s="31"/>
+      <c r="EJ1" s="31"/>
+      <c r="EK1" s="31"/>
+      <c r="EL1" s="31"/>
+      <c r="EM1" s="31"/>
     </row>
-    <row r="2" spans="2:144" ht="24.75" customHeight="1">
+    <row r="2" spans="2:144" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:144" ht="17.25" customHeight="1">
-      <c r="B3" s="39">
+    <row r="3" spans="2:144" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="32">
         <f ca="1">TODAY()-5</f>
-        <v>43898</v>
-      </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
+        <v>43899</v>
+      </c>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
     </row>
-    <row r="4" spans="2:144" s="18" customFormat="1" ht="18.75" customHeight="1">
+    <row r="4" spans="2:144" s="18" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="23"/>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
-      <c r="V4" s="30"/>
-      <c r="W4" s="30"/>
-      <c r="X4" s="30"/>
-      <c r="Y4" s="30"/>
-      <c r="Z4" s="30"/>
-      <c r="AA4" s="29" t="s">
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36"/>
+      <c r="Z4" s="36"/>
+      <c r="AA4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="AB4" s="29"/>
-      <c r="AC4" s="29"/>
-      <c r="AD4" s="29"/>
-      <c r="AE4" s="29"/>
-      <c r="AF4" s="29"/>
-      <c r="AG4" s="29"/>
-      <c r="AH4" s="29"/>
-      <c r="AI4" s="29"/>
-      <c r="AJ4" s="29"/>
-      <c r="AK4" s="29"/>
-      <c r="AL4" s="29"/>
-      <c r="AM4" s="29"/>
-      <c r="AN4" s="29"/>
-      <c r="AO4" s="29"/>
-      <c r="AP4" s="29"/>
-      <c r="AQ4" s="29"/>
-      <c r="AR4" s="29"/>
-      <c r="AS4" s="29"/>
-      <c r="AT4" s="29"/>
-      <c r="AU4" s="29"/>
-      <c r="AV4" s="29"/>
-      <c r="AW4" s="29"/>
-      <c r="AX4" s="29"/>
-      <c r="AY4" s="29"/>
-      <c r="AZ4" s="29"/>
-      <c r="BA4" s="29"/>
-      <c r="BB4" s="29"/>
-      <c r="BC4" s="29"/>
-      <c r="BD4" s="29"/>
-      <c r="BE4" s="33" t="s">
+      <c r="AB4" s="35"/>
+      <c r="AC4" s="35"/>
+      <c r="AD4" s="35"/>
+      <c r="AE4" s="35"/>
+      <c r="AF4" s="35"/>
+      <c r="AG4" s="35"/>
+      <c r="AH4" s="35"/>
+      <c r="AI4" s="35"/>
+      <c r="AJ4" s="35"/>
+      <c r="AK4" s="35"/>
+      <c r="AL4" s="35"/>
+      <c r="AM4" s="35"/>
+      <c r="AN4" s="35"/>
+      <c r="AO4" s="35"/>
+      <c r="AP4" s="35"/>
+      <c r="AQ4" s="35"/>
+      <c r="AR4" s="35"/>
+      <c r="AS4" s="35"/>
+      <c r="AT4" s="35"/>
+      <c r="AU4" s="35"/>
+      <c r="AV4" s="35"/>
+      <c r="AW4" s="35"/>
+      <c r="AX4" s="35"/>
+      <c r="AY4" s="35"/>
+      <c r="AZ4" s="35"/>
+      <c r="BA4" s="35"/>
+      <c r="BB4" s="35"/>
+      <c r="BC4" s="35"/>
+      <c r="BD4" s="35"/>
+      <c r="BE4" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="BF4" s="33"/>
-      <c r="BG4" s="33"/>
-      <c r="BH4" s="33"/>
-      <c r="BI4" s="33"/>
-      <c r="BJ4" s="33"/>
-      <c r="BK4" s="33"/>
-      <c r="BL4" s="33"/>
-      <c r="BM4" s="33"/>
-      <c r="BN4" s="33"/>
-      <c r="BO4" s="33"/>
-      <c r="BP4" s="33"/>
-      <c r="BQ4" s="33"/>
-      <c r="BR4" s="33"/>
-      <c r="BS4" s="33"/>
-      <c r="BT4" s="33"/>
-      <c r="BU4" s="33"/>
-      <c r="BV4" s="33"/>
-      <c r="BW4" s="33"/>
-      <c r="BX4" s="33"/>
-      <c r="BY4" s="33"/>
-      <c r="BZ4" s="33"/>
-      <c r="CA4" s="33"/>
-      <c r="CB4" s="33"/>
-      <c r="CC4" s="33"/>
-      <c r="CD4" s="33"/>
-      <c r="CE4" s="33"/>
-      <c r="CF4" s="33"/>
-      <c r="CG4" s="33"/>
-      <c r="CH4" s="33"/>
-      <c r="CI4" s="33"/>
-      <c r="CJ4" s="32" t="s">
+      <c r="BF4" s="39"/>
+      <c r="BG4" s="39"/>
+      <c r="BH4" s="39"/>
+      <c r="BI4" s="39"/>
+      <c r="BJ4" s="39"/>
+      <c r="BK4" s="39"/>
+      <c r="BL4" s="39"/>
+      <c r="BM4" s="39"/>
+      <c r="BN4" s="39"/>
+      <c r="BO4" s="39"/>
+      <c r="BP4" s="39"/>
+      <c r="BQ4" s="39"/>
+      <c r="BR4" s="39"/>
+      <c r="BS4" s="39"/>
+      <c r="BT4" s="39"/>
+      <c r="BU4" s="39"/>
+      <c r="BV4" s="39"/>
+      <c r="BW4" s="39"/>
+      <c r="BX4" s="39"/>
+      <c r="BY4" s="39"/>
+      <c r="BZ4" s="39"/>
+      <c r="CA4" s="39"/>
+      <c r="CB4" s="39"/>
+      <c r="CC4" s="39"/>
+      <c r="CD4" s="39"/>
+      <c r="CE4" s="39"/>
+      <c r="CF4" s="39"/>
+      <c r="CG4" s="39"/>
+      <c r="CH4" s="39"/>
+      <c r="CI4" s="39"/>
+      <c r="CJ4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="CK4" s="32"/>
-      <c r="CL4" s="32"/>
-      <c r="CM4" s="32"/>
-      <c r="CN4" s="32"/>
-      <c r="CO4" s="32"/>
-      <c r="CP4" s="32"/>
-      <c r="CQ4" s="32"/>
-      <c r="CR4" s="32"/>
-      <c r="CS4" s="32"/>
-      <c r="CT4" s="32"/>
-      <c r="CU4" s="32"/>
-      <c r="CV4" s="32"/>
-      <c r="CW4" s="32"/>
-      <c r="CX4" s="32"/>
-      <c r="CY4" s="32"/>
-      <c r="CZ4" s="32"/>
-      <c r="DA4" s="32"/>
-      <c r="DB4" s="32"/>
-      <c r="DC4" s="32"/>
-      <c r="DD4" s="32"/>
-      <c r="DE4" s="32"/>
-      <c r="DF4" s="32"/>
-      <c r="DG4" s="32"/>
-      <c r="DH4" s="32"/>
-      <c r="DI4" s="32"/>
-      <c r="DJ4" s="32"/>
-      <c r="DK4" s="32"/>
-      <c r="DL4" s="32"/>
-      <c r="DM4" s="32"/>
-      <c r="DN4" s="31" t="s">
+      <c r="CK4" s="38"/>
+      <c r="CL4" s="38"/>
+      <c r="CM4" s="38"/>
+      <c r="CN4" s="38"/>
+      <c r="CO4" s="38"/>
+      <c r="CP4" s="38"/>
+      <c r="CQ4" s="38"/>
+      <c r="CR4" s="38"/>
+      <c r="CS4" s="38"/>
+      <c r="CT4" s="38"/>
+      <c r="CU4" s="38"/>
+      <c r="CV4" s="38"/>
+      <c r="CW4" s="38"/>
+      <c r="CX4" s="38"/>
+      <c r="CY4" s="38"/>
+      <c r="CZ4" s="38"/>
+      <c r="DA4" s="38"/>
+      <c r="DB4" s="38"/>
+      <c r="DC4" s="38"/>
+      <c r="DD4" s="38"/>
+      <c r="DE4" s="38"/>
+      <c r="DF4" s="38"/>
+      <c r="DG4" s="38"/>
+      <c r="DH4" s="38"/>
+      <c r="DI4" s="38"/>
+      <c r="DJ4" s="38"/>
+      <c r="DK4" s="38"/>
+      <c r="DL4" s="38"/>
+      <c r="DM4" s="38"/>
+      <c r="DN4" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="DO4" s="31"/>
-      <c r="DP4" s="31"/>
-      <c r="DQ4" s="31"/>
-      <c r="DR4" s="31"/>
-      <c r="DS4" s="31"/>
-      <c r="DT4" s="31"/>
-      <c r="DU4" s="31"/>
-      <c r="DV4" s="31"/>
-      <c r="DW4" s="31"/>
-      <c r="DX4" s="31"/>
-      <c r="DY4" s="31"/>
-      <c r="DZ4" s="31"/>
-      <c r="EA4" s="31"/>
-      <c r="EB4" s="31"/>
-      <c r="EC4" s="31"/>
-      <c r="ED4" s="31"/>
-      <c r="EE4" s="31"/>
-      <c r="EF4" s="31"/>
-      <c r="EG4" s="31"/>
-      <c r="EH4" s="31"/>
-      <c r="EI4" s="31"/>
-      <c r="EJ4" s="31"/>
-      <c r="EK4" s="31"/>
-      <c r="EL4" s="31"/>
+      <c r="DO4" s="37"/>
+      <c r="DP4" s="37"/>
+      <c r="DQ4" s="37"/>
+      <c r="DR4" s="37"/>
+      <c r="DS4" s="37"/>
+      <c r="DT4" s="37"/>
+      <c r="DU4" s="37"/>
+      <c r="DV4" s="37"/>
+      <c r="DW4" s="37"/>
+      <c r="DX4" s="37"/>
+      <c r="DY4" s="37"/>
+      <c r="DZ4" s="37"/>
+      <c r="EA4" s="37"/>
+      <c r="EB4" s="37"/>
+      <c r="EC4" s="37"/>
+      <c r="ED4" s="37"/>
+      <c r="EE4" s="37"/>
+      <c r="EF4" s="37"/>
+      <c r="EG4" s="37"/>
+      <c r="EH4" s="37"/>
+      <c r="EI4" s="37"/>
+      <c r="EJ4" s="37"/>
+      <c r="EK4" s="37"/>
+      <c r="EL4" s="37"/>
       <c r="EM4" s="2"/>
       <c r="EN4" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:144" ht="24.75" customHeight="1">
+    <row r="5" spans="2:144" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="17"/>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="35" t="s">
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="34" t="s">
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
-      <c r="T5" s="34"/>
-      <c r="U5" s="34"/>
-      <c r="V5" s="34"/>
-      <c r="W5" s="34"/>
-      <c r="X5" s="35" t="s">
+      <c r="R5" s="33"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33"/>
+      <c r="U5" s="33"/>
+      <c r="V5" s="33"/>
+      <c r="W5" s="33"/>
+      <c r="X5" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="Y5" s="35"/>
-      <c r="Z5" s="35"/>
-      <c r="AA5" s="35"/>
-      <c r="AB5" s="35"/>
-      <c r="AC5" s="35"/>
-      <c r="AD5" s="35"/>
-      <c r="AE5" s="34" t="s">
+      <c r="Y5" s="34"/>
+      <c r="Z5" s="34"/>
+      <c r="AA5" s="34"/>
+      <c r="AB5" s="34"/>
+      <c r="AC5" s="34"/>
+      <c r="AD5" s="34"/>
+      <c r="AE5" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="AF5" s="34"/>
-      <c r="AG5" s="34"/>
-      <c r="AH5" s="34"/>
-      <c r="AI5" s="34"/>
-      <c r="AJ5" s="34"/>
-      <c r="AK5" s="34"/>
-      <c r="AL5" s="35" t="s">
+      <c r="AF5" s="33"/>
+      <c r="AG5" s="33"/>
+      <c r="AH5" s="33"/>
+      <c r="AI5" s="33"/>
+      <c r="AJ5" s="33"/>
+      <c r="AK5" s="33"/>
+      <c r="AL5" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AM5" s="35"/>
-      <c r="AN5" s="35"/>
-      <c r="AO5" s="35"/>
-      <c r="AP5" s="35"/>
-      <c r="AQ5" s="35"/>
-      <c r="AR5" s="35"/>
-      <c r="AS5" s="34" t="s">
+      <c r="AM5" s="34"/>
+      <c r="AN5" s="34"/>
+      <c r="AO5" s="34"/>
+      <c r="AP5" s="34"/>
+      <c r="AQ5" s="34"/>
+      <c r="AR5" s="34"/>
+      <c r="AS5" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="AT5" s="34"/>
-      <c r="AU5" s="34"/>
-      <c r="AV5" s="34"/>
-      <c r="AW5" s="34"/>
-      <c r="AX5" s="34"/>
-      <c r="AY5" s="34"/>
-      <c r="AZ5" s="35" t="s">
+      <c r="AT5" s="33"/>
+      <c r="AU5" s="33"/>
+      <c r="AV5" s="33"/>
+      <c r="AW5" s="33"/>
+      <c r="AX5" s="33"/>
+      <c r="AY5" s="33"/>
+      <c r="AZ5" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="BA5" s="35"/>
-      <c r="BB5" s="35"/>
-      <c r="BC5" s="35"/>
-      <c r="BD5" s="35"/>
-      <c r="BE5" s="35"/>
-      <c r="BF5" s="35"/>
-      <c r="BG5" s="34" t="s">
+      <c r="BA5" s="34"/>
+      <c r="BB5" s="34"/>
+      <c r="BC5" s="34"/>
+      <c r="BD5" s="34"/>
+      <c r="BE5" s="34"/>
+      <c r="BF5" s="34"/>
+      <c r="BG5" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="BH5" s="34"/>
-      <c r="BI5" s="34"/>
-      <c r="BJ5" s="34"/>
-      <c r="BK5" s="34"/>
-      <c r="BL5" s="34"/>
-      <c r="BM5" s="34"/>
-      <c r="BN5" s="35" t="s">
+      <c r="BH5" s="33"/>
+      <c r="BI5" s="33"/>
+      <c r="BJ5" s="33"/>
+      <c r="BK5" s="33"/>
+      <c r="BL5" s="33"/>
+      <c r="BM5" s="33"/>
+      <c r="BN5" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="BO5" s="35"/>
-      <c r="BP5" s="35"/>
-      <c r="BQ5" s="35"/>
-      <c r="BR5" s="35"/>
-      <c r="BS5" s="35"/>
-      <c r="BT5" s="35"/>
-      <c r="BU5" s="34" t="s">
+      <c r="BO5" s="34"/>
+      <c r="BP5" s="34"/>
+      <c r="BQ5" s="34"/>
+      <c r="BR5" s="34"/>
+      <c r="BS5" s="34"/>
+      <c r="BT5" s="34"/>
+      <c r="BU5" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="BV5" s="34"/>
-      <c r="BW5" s="34"/>
-      <c r="BX5" s="34"/>
-      <c r="BY5" s="34"/>
-      <c r="BZ5" s="34"/>
-      <c r="CA5" s="34"/>
-      <c r="CB5" s="35" t="s">
+      <c r="BV5" s="33"/>
+      <c r="BW5" s="33"/>
+      <c r="BX5" s="33"/>
+      <c r="BY5" s="33"/>
+      <c r="BZ5" s="33"/>
+      <c r="CA5" s="33"/>
+      <c r="CB5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="CC5" s="35"/>
-      <c r="CD5" s="35"/>
-      <c r="CE5" s="35"/>
-      <c r="CF5" s="35"/>
-      <c r="CG5" s="35"/>
-      <c r="CH5" s="35"/>
-      <c r="CI5" s="34" t="s">
+      <c r="CC5" s="34"/>
+      <c r="CD5" s="34"/>
+      <c r="CE5" s="34"/>
+      <c r="CF5" s="34"/>
+      <c r="CG5" s="34"/>
+      <c r="CH5" s="34"/>
+      <c r="CI5" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="CJ5" s="34"/>
-      <c r="CK5" s="34"/>
-      <c r="CL5" s="34"/>
-      <c r="CM5" s="34"/>
-      <c r="CN5" s="34"/>
-      <c r="CO5" s="34"/>
-      <c r="CP5" s="35" t="s">
+      <c r="CJ5" s="33"/>
+      <c r="CK5" s="33"/>
+      <c r="CL5" s="33"/>
+      <c r="CM5" s="33"/>
+      <c r="CN5" s="33"/>
+      <c r="CO5" s="33"/>
+      <c r="CP5" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="CQ5" s="35"/>
-      <c r="CR5" s="35"/>
-      <c r="CS5" s="35"/>
-      <c r="CT5" s="35"/>
-      <c r="CU5" s="35"/>
-      <c r="CV5" s="35"/>
-      <c r="CW5" s="34" t="s">
+      <c r="CQ5" s="34"/>
+      <c r="CR5" s="34"/>
+      <c r="CS5" s="34"/>
+      <c r="CT5" s="34"/>
+      <c r="CU5" s="34"/>
+      <c r="CV5" s="34"/>
+      <c r="CW5" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="CX5" s="34"/>
-      <c r="CY5" s="34"/>
-      <c r="CZ5" s="34"/>
-      <c r="DA5" s="34"/>
-      <c r="DB5" s="34"/>
-      <c r="DC5" s="34"/>
-      <c r="DD5" s="35" t="s">
+      <c r="CX5" s="33"/>
+      <c r="CY5" s="33"/>
+      <c r="CZ5" s="33"/>
+      <c r="DA5" s="33"/>
+      <c r="DB5" s="33"/>
+      <c r="DC5" s="33"/>
+      <c r="DD5" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="DE5" s="35"/>
-      <c r="DF5" s="35"/>
-      <c r="DG5" s="35"/>
-      <c r="DH5" s="35"/>
-      <c r="DI5" s="35"/>
-      <c r="DJ5" s="35"/>
-      <c r="DK5" s="34" t="s">
+      <c r="DE5" s="34"/>
+      <c r="DF5" s="34"/>
+      <c r="DG5" s="34"/>
+      <c r="DH5" s="34"/>
+      <c r="DI5" s="34"/>
+      <c r="DJ5" s="34"/>
+      <c r="DK5" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="DL5" s="34"/>
-      <c r="DM5" s="34"/>
-      <c r="DN5" s="34"/>
-      <c r="DO5" s="34"/>
-      <c r="DP5" s="34"/>
-      <c r="DQ5" s="34"/>
-      <c r="DR5" s="35" t="s">
+      <c r="DL5" s="33"/>
+      <c r="DM5" s="33"/>
+      <c r="DN5" s="33"/>
+      <c r="DO5" s="33"/>
+      <c r="DP5" s="33"/>
+      <c r="DQ5" s="33"/>
+      <c r="DR5" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="DS5" s="35"/>
-      <c r="DT5" s="35"/>
-      <c r="DU5" s="35"/>
-      <c r="DV5" s="35"/>
-      <c r="DW5" s="35"/>
-      <c r="DX5" s="35"/>
-      <c r="DY5" s="34" t="s">
+      <c r="DS5" s="34"/>
+      <c r="DT5" s="34"/>
+      <c r="DU5" s="34"/>
+      <c r="DV5" s="34"/>
+      <c r="DW5" s="34"/>
+      <c r="DX5" s="34"/>
+      <c r="DY5" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="DZ5" s="34"/>
-      <c r="EA5" s="34"/>
-      <c r="EB5" s="34"/>
-      <c r="EC5" s="34"/>
-      <c r="ED5" s="34"/>
-      <c r="EE5" s="34"/>
-      <c r="EF5" s="35" t="s">
+      <c r="DZ5" s="33"/>
+      <c r="EA5" s="33"/>
+      <c r="EB5" s="33"/>
+      <c r="EC5" s="33"/>
+      <c r="ED5" s="33"/>
+      <c r="EE5" s="33"/>
+      <c r="EF5" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="EG5" s="35"/>
-      <c r="EH5" s="35"/>
-      <c r="EI5" s="35"/>
-      <c r="EJ5" s="35"/>
-      <c r="EK5" s="35"/>
-      <c r="EL5" s="35"/>
-      <c r="EM5" s="36" t="s">
+      <c r="EG5" s="34"/>
+      <c r="EH5" s="34"/>
+      <c r="EI5" s="34"/>
+      <c r="EJ5" s="34"/>
+      <c r="EK5" s="34"/>
+      <c r="EL5" s="34"/>
+      <c r="EM5" s="29" t="s">
         <v>28</v>
       </c>
       <c r="EN5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:144" s="22" customFormat="1" ht="18" customHeight="1">
+    <row r="6" spans="2:144" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="26" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="19">
         <f ca="1">B3</f>
-        <v>43898</v>
+        <v>43899</v>
       </c>
       <c r="D6" s="19">
         <f ca="1">C6+1</f>
-        <v>43899</v>
+        <v>43900</v>
       </c>
       <c r="E6" s="19">
         <f t="shared" ref="E6:Q6" ca="1" si="0">D6+1</f>
-        <v>43900</v>
+        <v>43901</v>
       </c>
       <c r="F6" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>43901</v>
+        <v>43902</v>
       </c>
       <c r="G6" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>43902</v>
+        <v>43903</v>
       </c>
       <c r="H6" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>43903</v>
+        <v>43904</v>
       </c>
       <c r="I6" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>43904</v>
+        <v>43905</v>
       </c>
       <c r="J6" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>43905</v>
+        <v>43906</v>
       </c>
       <c r="K6" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>43906</v>
+        <v>43907</v>
       </c>
       <c r="L6" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>43907</v>
+        <v>43908</v>
       </c>
       <c r="M6" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>43908</v>
+        <v>43909</v>
       </c>
       <c r="N6" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>43909</v>
+        <v>43910</v>
       </c>
       <c r="O6" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>43910</v>
+        <v>43911</v>
       </c>
       <c r="P6" s="20">
         <f t="shared" ca="1" si="0"/>
-        <v>43911</v>
+        <v>43912</v>
       </c>
       <c r="Q6" s="21">
         <f t="shared" ca="1" si="0"/>
-        <v>43912</v>
+        <v>43913</v>
       </c>
       <c r="R6" s="21">
         <f t="shared" ref="R6:W6" ca="1" si="1">Q6+1</f>
-        <v>43913</v>
+        <v>43914</v>
       </c>
       <c r="S6" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>43914</v>
+        <v>43915</v>
       </c>
       <c r="T6" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>43915</v>
+        <v>43916</v>
       </c>
       <c r="U6" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>43916</v>
+        <v>43917</v>
       </c>
       <c r="V6" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>43917</v>
+        <v>43918</v>
       </c>
       <c r="W6" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="X6" s="20">
         <f t="shared" ref="X6" ca="1" si="2">W6+1</f>
-        <v>43919</v>
+        <v>43920</v>
       </c>
       <c r="Y6" s="20">
         <f t="shared" ref="Y6" ca="1" si="3">X6+1</f>
-        <v>43920</v>
+        <v>43921</v>
       </c>
       <c r="Z6" s="20">
         <f t="shared" ref="Z6" ca="1" si="4">Y6+1</f>
-        <v>43921</v>
+        <v>43922</v>
       </c>
       <c r="AA6" s="20">
         <f t="shared" ref="AA6" ca="1" si="5">Z6+1</f>
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="AB6" s="20">
         <f t="shared" ref="AB6" ca="1" si="6">AA6+1</f>
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="AC6" s="20">
         <f t="shared" ref="AC6" ca="1" si="7">AB6+1</f>
-        <v>43924</v>
+        <v>43925</v>
       </c>
       <c r="AD6" s="20">
         <f t="shared" ref="AD6" ca="1" si="8">AC6+1</f>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="AE6" s="19">
         <f ca="1">AD6+1</f>
-        <v>43926</v>
+        <v>43927</v>
       </c>
       <c r="AF6" s="19">
         <f ca="1">AE6+1</f>
-        <v>43927</v>
+        <v>43928</v>
       </c>
       <c r="AG6" s="19">
         <f t="shared" ref="AG6" ca="1" si="9">AF6+1</f>
-        <v>43928</v>
+        <v>43929</v>
       </c>
       <c r="AH6" s="19">
         <f t="shared" ref="AH6" ca="1" si="10">AG6+1</f>
-        <v>43929</v>
+        <v>43930</v>
       </c>
       <c r="AI6" s="19">
         <f t="shared" ref="AI6" ca="1" si="11">AH6+1</f>
-        <v>43930</v>
+        <v>43931</v>
       </c>
       <c r="AJ6" s="19">
         <f t="shared" ref="AJ6" ca="1" si="12">AI6+1</f>
-        <v>43931</v>
+        <v>43932</v>
       </c>
       <c r="AK6" s="19">
         <f t="shared" ref="AK6" ca="1" si="13">AJ6+1</f>
-        <v>43932</v>
+        <v>43933</v>
       </c>
       <c r="AL6" s="20">
         <f t="shared" ref="AL6" ca="1" si="14">AK6+1</f>
-        <v>43933</v>
+        <v>43934</v>
       </c>
       <c r="AM6" s="20">
         <f t="shared" ref="AM6" ca="1" si="15">AL6+1</f>
-        <v>43934</v>
+        <v>43935</v>
       </c>
       <c r="AN6" s="20">
         <f t="shared" ref="AN6" ca="1" si="16">AM6+1</f>
-        <v>43935</v>
+        <v>43936</v>
       </c>
       <c r="AO6" s="20">
         <f t="shared" ref="AO6" ca="1" si="17">AN6+1</f>
-        <v>43936</v>
+        <v>43937</v>
       </c>
       <c r="AP6" s="20">
         <f t="shared" ref="AP6" ca="1" si="18">AO6+1</f>
-        <v>43937</v>
+        <v>43938</v>
       </c>
       <c r="AQ6" s="20">
         <f t="shared" ref="AQ6" ca="1" si="19">AP6+1</f>
-        <v>43938</v>
+        <v>43939</v>
       </c>
       <c r="AR6" s="20">
         <f t="shared" ref="AR6" ca="1" si="20">AQ6+1</f>
-        <v>43939</v>
+        <v>43940</v>
       </c>
       <c r="AS6" s="19">
         <f ca="1">AR6+1</f>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="AT6" s="19">
         <f ca="1">AS6+1</f>
-        <v>43941</v>
+        <v>43942</v>
       </c>
       <c r="AU6" s="19">
         <f t="shared" ref="AU6" ca="1" si="21">AT6+1</f>
-        <v>43942</v>
+        <v>43943</v>
       </c>
       <c r="AV6" s="19">
         <f t="shared" ref="AV6" ca="1" si="22">AU6+1</f>
-        <v>43943</v>
+        <v>43944</v>
       </c>
       <c r="AW6" s="19">
         <f t="shared" ref="AW6" ca="1" si="23">AV6+1</f>
-        <v>43944</v>
+        <v>43945</v>
       </c>
       <c r="AX6" s="19">
         <f t="shared" ref="AX6" ca="1" si="24">AW6+1</f>
-        <v>43945</v>
+        <v>43946</v>
       </c>
       <c r="AY6" s="19">
         <f t="shared" ref="AY6" ca="1" si="25">AX6+1</f>
-        <v>43946</v>
+        <v>43947</v>
       </c>
       <c r="AZ6" s="20">
         <f ca="1">AY6+1</f>
-        <v>43947</v>
+        <v>43948</v>
       </c>
       <c r="BA6" s="20">
         <f t="shared" ref="BA6" ca="1" si="26">AZ6+1</f>
-        <v>43948</v>
+        <v>43949</v>
       </c>
       <c r="BB6" s="20">
         <f t="shared" ref="BB6" ca="1" si="27">BA6+1</f>
-        <v>43949</v>
+        <v>43950</v>
       </c>
       <c r="BC6" s="20">
         <f t="shared" ref="BC6" ca="1" si="28">BB6+1</f>
-        <v>43950</v>
+        <v>43951</v>
       </c>
       <c r="BD6" s="20">
         <f t="shared" ref="BD6" ca="1" si="29">BC6+1</f>
-        <v>43951</v>
+        <v>43952</v>
       </c>
       <c r="BE6" s="20">
         <f t="shared" ref="BE6" ca="1" si="30">BD6+1</f>
-        <v>43952</v>
+        <v>43953</v>
       </c>
       <c r="BF6" s="20">
         <f t="shared" ref="BF6" ca="1" si="31">BE6+1</f>
-        <v>43953</v>
+        <v>43954</v>
       </c>
       <c r="BG6" s="19">
         <f ca="1">BF6+1</f>
-        <v>43954</v>
+        <v>43955</v>
       </c>
       <c r="BH6" s="19">
         <f ca="1">BG6+1</f>
-        <v>43955</v>
+        <v>43956</v>
       </c>
       <c r="BI6" s="19">
         <f t="shared" ref="BI6" ca="1" si="32">BH6+1</f>
-        <v>43956</v>
+        <v>43957</v>
       </c>
       <c r="BJ6" s="19">
         <f t="shared" ref="BJ6" ca="1" si="33">BI6+1</f>
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="BK6" s="19">
         <f t="shared" ref="BK6" ca="1" si="34">BJ6+1</f>
-        <v>43958</v>
+        <v>43959</v>
       </c>
       <c r="BL6" s="19">
         <f t="shared" ref="BL6" ca="1" si="35">BK6+1</f>
-        <v>43959</v>
+        <v>43960</v>
       </c>
       <c r="BM6" s="19">
         <f t="shared" ref="BM6" ca="1" si="36">BL6+1</f>
-        <v>43960</v>
+        <v>43961</v>
       </c>
       <c r="BN6" s="20">
         <f ca="1">BM6+1</f>
-        <v>43961</v>
+        <v>43962</v>
       </c>
       <c r="BO6" s="20">
         <f t="shared" ref="BO6" ca="1" si="37">BN6+1</f>
-        <v>43962</v>
+        <v>43963</v>
       </c>
       <c r="BP6" s="20">
         <f t="shared" ref="BP6" ca="1" si="38">BO6+1</f>
-        <v>43963</v>
+        <v>43964</v>
       </c>
       <c r="BQ6" s="20">
         <f t="shared" ref="BQ6" ca="1" si="39">BP6+1</f>
-        <v>43964</v>
+        <v>43965</v>
       </c>
       <c r="BR6" s="20">
         <f t="shared" ref="BR6" ca="1" si="40">BQ6+1</f>
-        <v>43965</v>
+        <v>43966</v>
       </c>
       <c r="BS6" s="20">
         <f t="shared" ref="BS6" ca="1" si="41">BR6+1</f>
-        <v>43966</v>
+        <v>43967</v>
       </c>
       <c r="BT6" s="20">
         <f t="shared" ref="BT6" ca="1" si="42">BS6+1</f>
-        <v>43967</v>
+        <v>43968</v>
       </c>
       <c r="BU6" s="19">
         <f ca="1">BT6+1</f>
-        <v>43968</v>
+        <v>43969</v>
       </c>
       <c r="BV6" s="19">
         <f ca="1">BU6+1</f>
-        <v>43969</v>
+        <v>43970</v>
       </c>
       <c r="BW6" s="19">
         <f t="shared" ref="BW6" ca="1" si="43">BV6+1</f>
-        <v>43970</v>
+        <v>43971</v>
       </c>
       <c r="BX6" s="19">
         <f t="shared" ref="BX6" ca="1" si="44">BW6+1</f>
-        <v>43971</v>
+        <v>43972</v>
       </c>
       <c r="BY6" s="19">
         <f t="shared" ref="BY6" ca="1" si="45">BX6+1</f>
-        <v>43972</v>
+        <v>43973</v>
       </c>
       <c r="BZ6" s="19">
         <f t="shared" ref="BZ6" ca="1" si="46">BY6+1</f>
-        <v>43973</v>
+        <v>43974</v>
       </c>
       <c r="CA6" s="19">
         <f t="shared" ref="CA6" ca="1" si="47">BZ6+1</f>
-        <v>43974</v>
+        <v>43975</v>
       </c>
       <c r="CB6" s="20">
         <f t="shared" ref="CB6" ca="1" si="48">CA6+1</f>
-        <v>43975</v>
+        <v>43976</v>
       </c>
       <c r="CC6" s="20">
         <f t="shared" ref="CC6" ca="1" si="49">CB6+1</f>
-        <v>43976</v>
+        <v>43977</v>
       </c>
       <c r="CD6" s="20">
         <f t="shared" ref="CD6" ca="1" si="50">CC6+1</f>
-        <v>43977</v>
+        <v>43978</v>
       </c>
       <c r="CE6" s="20">
         <f t="shared" ref="CE6" ca="1" si="51">CD6+1</f>
-        <v>43978</v>
+        <v>43979</v>
       </c>
       <c r="CF6" s="20">
         <f t="shared" ref="CF6" ca="1" si="52">CE6+1</f>
-        <v>43979</v>
+        <v>43980</v>
       </c>
       <c r="CG6" s="20">
         <f t="shared" ref="CG6" ca="1" si="53">CF6+1</f>
-        <v>43980</v>
+        <v>43981</v>
       </c>
       <c r="CH6" s="20">
         <f t="shared" ref="CH6" ca="1" si="54">CG6+1</f>
-        <v>43981</v>
+        <v>43982</v>
       </c>
       <c r="CI6" s="19">
         <f ca="1">CH6+1</f>
-        <v>43982</v>
+        <v>43983</v>
       </c>
       <c r="CJ6" s="19">
         <f ca="1">CI6+1</f>
-        <v>43983</v>
+        <v>43984</v>
       </c>
       <c r="CK6" s="19">
         <f t="shared" ref="CK6" ca="1" si="55">CJ6+1</f>
-        <v>43984</v>
+        <v>43985</v>
       </c>
       <c r="CL6" s="19">
         <f t="shared" ref="CL6" ca="1" si="56">CK6+1</f>
-        <v>43985</v>
+        <v>43986</v>
       </c>
       <c r="CM6" s="19">
         <f t="shared" ref="CM6" ca="1" si="57">CL6+1</f>
-        <v>43986</v>
+        <v>43987</v>
       </c>
       <c r="CN6" s="19">
         <f t="shared" ref="CN6" ca="1" si="58">CM6+1</f>
-        <v>43987</v>
+        <v>43988</v>
       </c>
       <c r="CO6" s="19">
         <f t="shared" ref="CO6" ca="1" si="59">CN6+1</f>
-        <v>43988</v>
+        <v>43989</v>
       </c>
       <c r="CP6" s="20">
         <f t="shared" ref="CP6" ca="1" si="60">CO6+1</f>
-        <v>43989</v>
+        <v>43990</v>
       </c>
       <c r="CQ6" s="20">
         <f t="shared" ref="CQ6" ca="1" si="61">CP6+1</f>
-        <v>43990</v>
+        <v>43991</v>
       </c>
       <c r="CR6" s="20">
         <f t="shared" ref="CR6" ca="1" si="62">CQ6+1</f>
-        <v>43991</v>
+        <v>43992</v>
       </c>
       <c r="CS6" s="20">
         <f t="shared" ref="CS6" ca="1" si="63">CR6+1</f>
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="CT6" s="20">
         <f t="shared" ref="CT6" ca="1" si="64">CS6+1</f>
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="CU6" s="20">
         <f t="shared" ref="CU6" ca="1" si="65">CT6+1</f>
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="CV6" s="20">
         <f t="shared" ref="CV6" ca="1" si="66">CU6+1</f>
-        <v>43995</v>
+        <v>43996</v>
       </c>
       <c r="CW6" s="19">
         <f ca="1">CV6+1</f>
-        <v>43996</v>
+        <v>43997</v>
       </c>
       <c r="CX6" s="19">
         <f ca="1">CW6+1</f>
-        <v>43997</v>
+        <v>43998</v>
       </c>
       <c r="CY6" s="19">
         <f t="shared" ref="CY6" ca="1" si="67">CX6+1</f>
-        <v>43998</v>
+        <v>43999</v>
       </c>
       <c r="CZ6" s="19">
         <f t="shared" ref="CZ6" ca="1" si="68">CY6+1</f>
-        <v>43999</v>
+        <v>44000</v>
       </c>
       <c r="DA6" s="19">
         <f t="shared" ref="DA6" ca="1" si="69">CZ6+1</f>
-        <v>44000</v>
+        <v>44001</v>
       </c>
       <c r="DB6" s="19">
         <f t="shared" ref="DB6" ca="1" si="70">DA6+1</f>
-        <v>44001</v>
+        <v>44002</v>
       </c>
       <c r="DC6" s="19">
         <f t="shared" ref="DC6" ca="1" si="71">DB6+1</f>
-        <v>44002</v>
+        <v>44003</v>
       </c>
       <c r="DD6" s="20">
         <f ca="1">DC6+1</f>
-        <v>44003</v>
+        <v>44004</v>
       </c>
       <c r="DE6" s="20">
         <f t="shared" ref="DE6" ca="1" si="72">DD6+1</f>
-        <v>44004</v>
+        <v>44005</v>
       </c>
       <c r="DF6" s="20">
         <f t="shared" ref="DF6" ca="1" si="73">DE6+1</f>
-        <v>44005</v>
+        <v>44006</v>
       </c>
       <c r="DG6" s="20">
         <f t="shared" ref="DG6" ca="1" si="74">DF6+1</f>
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="DH6" s="20">
         <f t="shared" ref="DH6" ca="1" si="75">DG6+1</f>
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="DI6" s="20">
         <f t="shared" ref="DI6" ca="1" si="76">DH6+1</f>
-        <v>44008</v>
+        <v>44009</v>
       </c>
       <c r="DJ6" s="20">
         <f t="shared" ref="DJ6" ca="1" si="77">DI6+1</f>
-        <v>44009</v>
+        <v>44010</v>
       </c>
       <c r="DK6" s="19">
         <f ca="1">DJ6+1</f>
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="DL6" s="19">
         <f ca="1">DK6+1</f>
-        <v>44011</v>
+        <v>44012</v>
       </c>
       <c r="DM6" s="19">
         <f t="shared" ref="DM6" ca="1" si="78">DL6+1</f>
-        <v>44012</v>
+        <v>44013</v>
       </c>
       <c r="DN6" s="19">
         <f t="shared" ref="DN6" ca="1" si="79">DM6+1</f>
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="DO6" s="19">
         <f t="shared" ref="DO6" ca="1" si="80">DN6+1</f>
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="DP6" s="19">
         <f t="shared" ref="DP6" ca="1" si="81">DO6+1</f>
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="DQ6" s="19">
         <f t="shared" ref="DQ6" ca="1" si="82">DP6+1</f>
-        <v>44016</v>
+        <v>44017</v>
       </c>
       <c r="DR6" s="20">
         <f t="shared" ref="DR6" ca="1" si="83">DQ6+1</f>
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="DS6" s="20">
         <f t="shared" ref="DS6" ca="1" si="84">DR6+1</f>
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="DT6" s="20">
         <f t="shared" ref="DT6" ca="1" si="85">DS6+1</f>
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="DU6" s="20">
         <f t="shared" ref="DU6" ca="1" si="86">DT6+1</f>
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="DV6" s="20">
         <f t="shared" ref="DV6" ca="1" si="87">DU6+1</f>
-        <v>44021</v>
+        <v>44022</v>
       </c>
       <c r="DW6" s="20">
         <f t="shared" ref="DW6" ca="1" si="88">DV6+1</f>
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="DX6" s="20">
         <f t="shared" ref="DX6" ca="1" si="89">DW6+1</f>
-        <v>44023</v>
+        <v>44024</v>
       </c>
       <c r="DY6" s="19">
         <f ca="1">DX6+1</f>
-        <v>44024</v>
+        <v>44025</v>
       </c>
       <c r="DZ6" s="19">
         <f ca="1">DY6+1</f>
-        <v>44025</v>
+        <v>44026</v>
       </c>
       <c r="EA6" s="19">
         <f t="shared" ref="EA6" ca="1" si="90">DZ6+1</f>
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="EB6" s="19">
         <f t="shared" ref="EB6" ca="1" si="91">EA6+1</f>
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="EC6" s="19">
         <f t="shared" ref="EC6" ca="1" si="92">EB6+1</f>
-        <v>44028</v>
+        <v>44029</v>
       </c>
       <c r="ED6" s="19">
         <f t="shared" ref="ED6" ca="1" si="93">EC6+1</f>
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="EE6" s="19">
         <f t="shared" ref="EE6" ca="1" si="94">ED6+1</f>
-        <v>44030</v>
+        <v>44031</v>
       </c>
       <c r="EF6" s="20">
         <f ca="1">EE6+1</f>
-        <v>44031</v>
+        <v>44032</v>
       </c>
       <c r="EG6" s="20">
         <f t="shared" ref="EG6" ca="1" si="95">EF6+1</f>
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="EH6" s="20">
         <f t="shared" ref="EH6" ca="1" si="96">EG6+1</f>
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="EI6" s="20">
         <f t="shared" ref="EI6" ca="1" si="97">EH6+1</f>
-        <v>44034</v>
+        <v>44035</v>
       </c>
       <c r="EJ6" s="20">
         <f t="shared" ref="EJ6" ca="1" si="98">EI6+1</f>
-        <v>44035</v>
+        <v>44036</v>
       </c>
       <c r="EK6" s="20">
         <f t="shared" ref="EK6" ca="1" si="99">EJ6+1</f>
-        <v>44036</v>
+        <v>44037</v>
       </c>
       <c r="EL6" s="20">
         <f t="shared" ref="EL6" ca="1" si="100">EK6+1</f>
-        <v>44037</v>
-      </c>
-      <c r="EM6" s="37"/>
+        <v>44038</v>
+      </c>
+      <c r="EM6" s="30"/>
     </row>
-    <row r="7" spans="2:144" ht="45" customHeight="1">
+    <row r="7" spans="2:144" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="27" t="s">
         <v>30</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="2:144" ht="32.25" customHeight="1">
+    <row r="8" spans="2:144" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="27" t="s">
         <v>32</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:144" ht="30" customHeight="1">
+    <row r="9" spans="2:144" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="27" t="s">
         <v>34</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="2:144" ht="30" customHeight="1">
+    <row r="10" spans="2:144" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="27" t="s">
         <v>36</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="2:144" ht="35.25" customHeight="1">
+    <row r="11" spans="2:144" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="27" t="s">
         <v>38</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="2:144" ht="37.5" customHeight="1">
+    <row r="12" spans="2:144" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="27" t="s">
         <v>40</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="2:144" ht="42.75" customHeight="1">
+    <row r="13" spans="2:144" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="27" t="s">
         <v>41</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="2:144" ht="66.75" customHeight="1">
+    <row r="14" spans="2:144" ht="66.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="27" t="s">
         <v>43</v>
       </c>
@@ -3827,9 +3827,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="2:144" ht="30" customHeight="1">
+    <row r="15" spans="2:144" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="27" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
@@ -3975,9 +3975,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="2:144" ht="30" customHeight="1">
+    <row r="16" spans="2:144" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
@@ -4123,9 +4123,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="2:143" ht="45" customHeight="1">
+    <row r="17" spans="2:143" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
@@ -4268,12 +4268,12 @@
       <c r="EK17" s="5"/>
       <c r="EL17" s="6"/>
       <c r="EM17" s="28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="2:143" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="27" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="2:143" ht="30" customHeight="1">
-      <c r="B18" s="27" t="s">
-        <v>48</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
@@ -4416,12 +4416,12 @@
       <c r="EK18" s="5"/>
       <c r="EL18" s="6"/>
       <c r="EM18" s="28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="2:143" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="27" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="2:143" ht="43.5" customHeight="1">
-      <c r="B19" s="27" t="s">
-        <v>50</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
@@ -4564,12 +4564,12 @@
       <c r="EK19" s="5"/>
       <c r="EL19" s="6"/>
       <c r="EM19" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="20" spans="2:143" ht="30" customHeight="1">
+    <row r="20" spans="2:143" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
@@ -4715,9 +4715,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="2:143" ht="30" customHeight="1">
+    <row r="21" spans="2:143" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
@@ -4863,9 +4863,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="2:143" ht="30" customHeight="1">
+    <row r="22" spans="2:143" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
@@ -5008,12 +5008,12 @@
       <c r="EK22" s="9"/>
       <c r="EL22" s="10"/>
       <c r="EM22" s="28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="2:143" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="27" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="2:143" ht="30" customHeight="1">
-      <c r="B23" s="27" t="s">
-        <v>55</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
@@ -5156,12 +5156,12 @@
       <c r="EK23" s="5"/>
       <c r="EL23" s="6"/>
       <c r="EM23" s="28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:143" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="27" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="2:143" ht="30" customHeight="1">
-      <c r="B24" s="27" t="s">
-        <v>57</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
@@ -5304,12 +5304,12 @@
       <c r="EK24" s="9"/>
       <c r="EL24" s="10"/>
       <c r="EM24" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="2:143" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="27" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="2:143" ht="30" customHeight="1">
-      <c r="B25" s="27" t="s">
-        <v>59</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="6"/>
@@ -5455,9 +5455,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="2:143" ht="55.5" customHeight="1">
+    <row r="26" spans="2:143" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
@@ -5603,9 +5603,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="2:143" ht="45" customHeight="1">
+    <row r="27" spans="2:143" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
@@ -5751,9 +5751,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="2:143" ht="30" customHeight="1">
+    <row r="28" spans="2:143" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="24"/>
       <c r="D28" s="25"/>
@@ -5899,9 +5899,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="2:143" ht="30" customHeight="1">
+    <row r="29" spans="2:143" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" s="24"/>
       <c r="D29" s="25"/>
@@ -6049,6 +6049,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="AA4:BD4"/>
+    <mergeCell ref="C4:Z4"/>
+    <mergeCell ref="DN4:EL4"/>
+    <mergeCell ref="CJ4:DM4"/>
+    <mergeCell ref="BE4:CI4"/>
+    <mergeCell ref="DY5:EE5"/>
+    <mergeCell ref="EF5:EL5"/>
+    <mergeCell ref="CB5:CH5"/>
+    <mergeCell ref="CI5:CO5"/>
+    <mergeCell ref="CP5:CV5"/>
+    <mergeCell ref="CW5:DC5"/>
+    <mergeCell ref="DD5:DJ5"/>
     <mergeCell ref="EM5:EM6"/>
     <mergeCell ref="B1:EM1"/>
     <mergeCell ref="B3:D3"/>
@@ -6065,18 +6077,6 @@
     <mergeCell ref="BU5:CA5"/>
     <mergeCell ref="DK5:DQ5"/>
     <mergeCell ref="DR5:DX5"/>
-    <mergeCell ref="DY5:EE5"/>
-    <mergeCell ref="EF5:EL5"/>
-    <mergeCell ref="CB5:CH5"/>
-    <mergeCell ref="CI5:CO5"/>
-    <mergeCell ref="CP5:CV5"/>
-    <mergeCell ref="CW5:DC5"/>
-    <mergeCell ref="DD5:DJ5"/>
-    <mergeCell ref="AA4:BD4"/>
-    <mergeCell ref="C4:Z4"/>
-    <mergeCell ref="DN4:EL4"/>
-    <mergeCell ref="CJ4:DM4"/>
-    <mergeCell ref="BE4:CI4"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:W6">
     <cfRule type="expression" dxfId="17" priority="20">

</xml_diff>